<commit_message>
SQL DML - Finish refresh test data - 28.11.2023
</commit_message>
<xml_diff>
--- a/1. Database Design/JAVA 19 20 - Quyen Phan - Database Design.xlsx
+++ b/1. Database Design/JAVA 19 20 - Quyen Phan - Database Design.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E895BA-B6EF-4227-A7D9-DFA141F44584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC69F2A-F7F3-4861-9D2A-0C3112B550D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="883" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="883" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="396">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -1581,9 +1581,6 @@
     <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5) --&gt; Nhân viên 3</t>
   </si>
   <si>
-    <t xml:space="preserve"> -- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7) --&gt; Nhân viên 4</t>
-  </si>
-  <si>
     <t>INSERT INTO `order_delivery_status_detail`(ORDER_ID, STATUS_ID, EMPLOYEE_ID, LAST_UPDATED_AT)</t>
   </si>
   <si>
@@ -1723,6 +1720,18 @@
   </si>
   <si>
     <t>T13x</t>
+  </si>
+  <si>
+    <t>T04 x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 1, 7) --&gt; Nhân viên 4</t>
+  </si>
+  <si>
+    <t>T07 x</t>
+  </si>
+  <si>
+    <t>T08 x</t>
   </si>
 </sst>
 </file>
@@ -2962,10 +2971,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1E66AC-B7AB-4694-9C29-CBC315CB6160}">
-  <dimension ref="B1:E52"/>
+  <dimension ref="B1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,14 +2987,14 @@
     <col min="6" max="29" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>72</v>
       </c>
@@ -2999,7 +3008,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="43">
         <v>1</v>
       </c>
@@ -3012,8 +3021,12 @@
       <c r="E5" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f>'B4. Cơ sở dữ liệu vật lý'!E5 'B4. Cơ sở dữ liệu vật lý'!E5</f>
+        <v>T04 x</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="43">
         <v>2</v>
       </c>
@@ -3026,8 +3039,12 @@
       <c r="E6" s="56">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F52" si="0">_xlfn.CONCAT("(",B6,",",C6,",",D6,",",E6,")",",")</f>
+        <v>(2,1,31,5),</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="43">
         <v>3</v>
       </c>
@@ -3040,8 +3057,12 @@
       <c r="E7" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,1,49,1),</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="43">
         <v>4</v>
       </c>
@@ -3054,8 +3075,12 @@
       <c r="E8" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,1,68,2),</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="43">
         <v>5</v>
       </c>
@@ -3068,8 +3093,12 @@
       <c r="E9" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,2,39,2),</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="43">
         <v>6</v>
       </c>
@@ -3082,8 +3111,12 @@
       <c r="E10" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,2,48,2),</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="43">
         <v>7</v>
       </c>
@@ -3096,8 +3129,12 @@
       <c r="E11" s="56">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,2,50,12),</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="43">
         <v>8</v>
       </c>
@@ -3110,8 +3147,12 @@
       <c r="E12" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,2,53,3),</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="43">
         <v>9</v>
       </c>
@@ -3124,8 +3165,12 @@
       <c r="E13" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,3,21,2),</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="43">
         <v>10</v>
       </c>
@@ -3138,8 +3183,12 @@
       <c r="E14" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,3,22,2),</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="43">
         <v>11</v>
       </c>
@@ -3152,8 +3201,12 @@
       <c r="E15" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,3,39,2),</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="43">
         <v>12</v>
       </c>
@@ -3166,8 +3219,12 @@
       <c r="E16" s="56">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,3,49,11),</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="43">
         <v>13</v>
       </c>
@@ -3180,8 +3237,12 @@
       <c r="E17" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,4,11,2),</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="43">
         <v>14</v>
       </c>
@@ -3194,8 +3255,12 @@
       <c r="E18" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,4,41,3),</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="43">
         <v>15</v>
       </c>
@@ -3208,8 +3273,12 @@
       <c r="E19" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,4,46,3),</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="43">
         <v>16</v>
       </c>
@@ -3222,8 +3291,12 @@
       <c r="E20" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,4,69,3),</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="43">
         <v>17</v>
       </c>
@@ -3236,8 +3309,12 @@
       <c r="E21" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,5,5,3),</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="43">
         <v>18</v>
       </c>
@@ -3250,8 +3327,12 @@
       <c r="E22" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,5,24,2),</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="43">
         <v>19</v>
       </c>
@@ -3264,8 +3345,12 @@
       <c r="E23" s="56">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,5,39,8),</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="43">
         <v>20</v>
       </c>
@@ -3278,8 +3363,12 @@
       <c r="E24" s="56">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,5,56,8),</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="43">
         <v>21</v>
       </c>
@@ -3292,8 +3381,12 @@
       <c r="E25" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,6,10,2),</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="43">
         <v>22</v>
       </c>
@@ -3306,8 +3399,12 @@
       <c r="E26" s="56">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,6,23,9),</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="43">
         <v>23</v>
       </c>
@@ -3320,8 +3417,12 @@
       <c r="E27" s="56">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,6,29,3),</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="43">
         <v>24</v>
       </c>
@@ -3334,8 +3435,12 @@
       <c r="E28" s="56">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,6,30,11),</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="43">
         <v>25</v>
       </c>
@@ -3348,8 +3453,12 @@
       <c r="E29" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,7,17,2),</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="43">
         <v>26</v>
       </c>
@@ -3362,8 +3471,12 @@
       <c r="E30" s="56">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,7,43,15),</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="43">
         <v>27</v>
       </c>
@@ -3376,8 +3489,12 @@
       <c r="E31" s="56">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,7,54,10),</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="43">
         <v>28</v>
       </c>
@@ -3390,8 +3507,12 @@
       <c r="E32" s="56">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,7,57,5),</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="43">
         <v>29</v>
       </c>
@@ -3404,8 +3525,12 @@
       <c r="E33" s="56">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,8,8,20),</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="43">
         <v>30</v>
       </c>
@@ -3418,8 +3543,12 @@
       <c r="E34" s="56">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,8,18,7),</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="43">
         <v>31</v>
       </c>
@@ -3432,8 +3561,12 @@
       <c r="E35" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,8,59,2),</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="43">
         <v>32</v>
       </c>
@@ -3446,8 +3579,12 @@
       <c r="E36" s="56">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,8,65,9),</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="43">
         <v>33</v>
       </c>
@@ -3460,8 +3597,12 @@
       <c r="E37" s="56">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>(33,9,29,10),</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="43">
         <v>34</v>
       </c>
@@ -3474,8 +3615,12 @@
       <c r="E38" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>(34,9,34,1),</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="43">
         <v>35</v>
       </c>
@@ -3488,8 +3633,12 @@
       <c r="E39" s="56">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>(35,9,38,7),</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="43">
         <v>36</v>
       </c>
@@ -3502,8 +3651,12 @@
       <c r="E40" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>(36,9,53,2),</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="43">
         <v>37</v>
       </c>
@@ -3516,8 +3669,12 @@
       <c r="E41" s="56">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>(37,10,22,10),</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="43">
         <v>38</v>
       </c>
@@ -3530,8 +3687,12 @@
       <c r="E42" s="56">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>(38,10,24,10),</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="43">
         <v>39</v>
       </c>
@@ -3544,8 +3705,12 @@
       <c r="E43" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>(39,10,40,2),</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="43">
         <v>40</v>
       </c>
@@ -3558,8 +3723,12 @@
       <c r="E44" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>(40,10,50,2),</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="43">
         <v>41</v>
       </c>
@@ -3572,8 +3741,12 @@
       <c r="E45" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>(41,11,37,2),</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="43">
         <v>42</v>
       </c>
@@ -3586,8 +3759,12 @@
       <c r="E46" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>(42,11,38,2),</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="43">
         <v>43</v>
       </c>
@@ -3600,8 +3777,12 @@
       <c r="E47" s="56">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>(43,11,48,11),</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="43">
         <v>44</v>
       </c>
@@ -3614,8 +3795,12 @@
       <c r="E48" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>(44,11,51,2),</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="43">
         <v>45</v>
       </c>
@@ -3628,8 +3813,12 @@
       <c r="E49" s="56">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>(45,12,1,12),</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="43">
         <v>46</v>
       </c>
@@ -3642,8 +3831,12 @@
       <c r="E50" s="56">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>(46,12,29,2),</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="43">
         <v>47</v>
       </c>
@@ -3656,8 +3849,12 @@
       <c r="E51" s="56">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>(47,12,35,1),</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="43">
         <v>48</v>
       </c>
@@ -3669,6 +3866,10 @@
       </c>
       <c r="E52" s="56">
         <v>3</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>(48,12,42,3),</v>
       </c>
     </row>
   </sheetData>
@@ -3998,8 +4199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B2115A-D7BF-41E7-AB58-A59A037F38B4}">
   <dimension ref="B1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4057,7 +4258,7 @@
     </row>
     <row r="9" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="63" t="s">
-        <v>345</v>
+        <v>393</v>
       </c>
       <c r="C9" s="64"/>
     </row>
@@ -4071,17 +4272,17 @@
     <row r="13" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="62" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4091,53 +4292,53 @@
     </row>
     <row r="18" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4147,37 +4348,37 @@
     </row>
     <row r="30" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="36" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4189,7 +4390,7 @@
     <row r="38" spans="3:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
@@ -4199,37 +4400,37 @@
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -4240,60 +4441,60 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
+        <v>372</v>
+      </c>
+      <c r="D59" t="s">
         <v>373</v>
-      </c>
-      <c r="D59" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -4836,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD1D9A7-6595-4AD7-8E58-C4F147702EF9}">
   <dimension ref="B3:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4881,7 +5082,7 @@
         <v>210</v>
       </c>
       <c r="G5" s="62" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6221,7 +6422,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="57" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8634,8 +8835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79120E3-8B85-45B8-906C-9F3770585442}">
   <dimension ref="A1:Y142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -8706,43 +8907,43 @@
     </row>
     <row r="5" spans="2:25" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>380</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>379</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="H5" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="K5" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="18" t="s">
+      <c r="L5" s="18" t="s">
         <v>389</v>
       </c>
-      <c r="K5" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="L5" s="18" t="s">
+      <c r="M5" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="N5" s="18" t="s">
         <v>391</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>392</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
@@ -11261,7 +11462,7 @@
         <v>72</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>89</v>
@@ -11359,7 +11560,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F8" s="57">
         <v>2</v>
@@ -11382,7 +11583,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F9" s="57">
         <v>3</v>

</xml_diff>